<commit_message>
v0.0.1 CHANGE: The format of docstrings CHANGE: Variable names ADD: A bunch of printing lines
</commit_message>
<xml_diff>
--- a/浙江省2019年三位一体招生信息.xlsx
+++ b/浙江省2019年三位一体招生信息.xlsx
@@ -1,13 +1,13 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+<workbook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <workbookPr/>
   <workbookProtection/>
   <bookViews>
     <workbookView activeTab="0" autoFilterDateGrouping="1" firstSheet="0" minimized="0" showHorizontalScroll="1" showSheetTabs="1" showVerticalScroll="1" tabRatio="600" visibility="visible"/>
   </bookViews>
   <sheets>
-    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="报考简章" sheetId="1" state="visible" r:id="rId1"/>
+    <sheet name="报考简章" sheetId="1" state="visible" r:id="rId1"/>
   </sheets>
   <definedNames/>
   <calcPr calcId="124519" fullCalcOnLoad="1"/>

</xml_diff>

<commit_message>
v0.0.2 - ADD: Update README.md - CHANGE: Delete some useless files
</commit_message>
<xml_diff>
--- a/浙江省2019年三位一体招生信息.xlsx
+++ b/浙江省2019年三位一体招生信息.xlsx
@@ -1,21 +1,26 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="21001"/>
   <workbookPr/>
-  <workbookProtection/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Vanad\OneDrive\Documents\Computer Science\Python\Projects\2019-zhejiang-universities-admission-info-scraper\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="1" documentId="11_083E72B50EBA80104345557E01FB694A8904A63C" xr6:coauthVersionLast="38" xr6:coauthVersionMax="38" xr10:uidLastSave="{56898ED1-A20A-4BCB-9195-8D1D41F5DCED}"/>
   <bookViews>
-    <workbookView activeTab="0" autoFilterDateGrouping="1" firstSheet="0" minimized="0" showHorizontalScroll="1" showSheetTabs="1" showVerticalScroll="1" tabRatio="600" visibility="visible"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="22500" windowHeight="12330" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
-    <sheet name="报考简章" sheetId="1" state="visible" r:id="rId1"/>
+    <sheet name="报考简章" sheetId="1" r:id="rId1"/>
   </sheets>
-  <definedNames/>
-  <calcPr calcId="124519" fullCalcOnLoad="1"/>
+  <calcPr calcId="0"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="142">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="150" uniqueCount="142">
   <si>
     <t>高校名单</t>
   </si>
@@ -446,20 +451,27 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <numFmts count="0"/>
-  <fonts count="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
+      <sz val="11"/>
+      <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
-      <color theme="1"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
       <sz val="11"/>
+      <color theme="10"/>
+      <name val="Calibri"/>
+      <family val="2"/>
       <scheme val="minor"/>
     </font>
   </fonts>
   <fills count="2">
     <fill>
-      <patternFill/>
+      <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
@@ -474,16 +486,28 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="1">
-    <xf borderId="0" fillId="0" fontId="0" numFmtId="0"/>
+  <cellStyleXfs count="2">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
-    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
+  <cellXfs count="2">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1"/>
   </cellXfs>
-  <cellStyles count="1">
-    <cellStyle builtinId="0" hidden="0" name="Normal" xfId="0"/>
+  <cellStyles count="2">
+    <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
+    <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <tableStyles count="0" defaultPivotStyle="PivotStyleLight16" defaultTableStyle="TableStyleMedium9"/>
+  <dxfs count="0"/>
+  <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
+      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
+    </ext>
+  </extLst>
 </styleSheet>
 </file>
 
@@ -771,20 +795,16 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <sheetPr>
-    <outlinePr summaryBelow="1" summaryRight="1"/>
-    <pageSetUpPr/>
-  </sheetPr>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:C50"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A1" sqref="A1"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C2" sqref="C2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
   <sheetData>
-    <row r="1" spans="1:3">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -795,18 +815,18 @@
         <v>2</v>
       </c>
     </row>
-    <row r="2" spans="1:3">
+    <row r="2" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A2" t="s">
         <v>3</v>
       </c>
       <c r="B2" t="s">
         <v>4</v>
       </c>
-      <c r="C2" t="s">
+      <c r="C2" s="1" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="3" spans="1:3">
+    <row r="3" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A3" t="s">
         <v>6</v>
       </c>
@@ -817,7 +837,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="4" spans="1:3">
+    <row r="4" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A4" t="s">
         <v>9</v>
       </c>
@@ -828,7 +848,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="5" spans="1:3">
+    <row r="5" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A5" t="s">
         <v>12</v>
       </c>
@@ -839,7 +859,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="6" spans="1:3">
+    <row r="6" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A6" t="s">
         <v>15</v>
       </c>
@@ -850,7 +870,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="7" spans="1:3">
+    <row r="7" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A7" t="s">
         <v>18</v>
       </c>
@@ -861,7 +881,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="8" spans="1:3">
+    <row r="8" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A8" t="s">
         <v>21</v>
       </c>
@@ -872,7 +892,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="9" spans="1:3">
+    <row r="9" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A9" t="s">
         <v>24</v>
       </c>
@@ -883,7 +903,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="10" spans="1:3">
+    <row r="10" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A10" t="s">
         <v>27</v>
       </c>
@@ -894,7 +914,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="11" spans="1:3">
+    <row r="11" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A11" t="s">
         <v>30</v>
       </c>
@@ -905,7 +925,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="12" spans="1:3">
+    <row r="12" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A12" t="s">
         <v>32</v>
       </c>
@@ -916,7 +936,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="13" spans="1:3">
+    <row r="13" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A13" t="s">
         <v>35</v>
       </c>
@@ -927,7 +947,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="14" spans="1:3">
+    <row r="14" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A14" t="s">
         <v>38</v>
       </c>
@@ -938,7 +958,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="15" spans="1:3">
+    <row r="15" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A15" t="s">
         <v>41</v>
       </c>
@@ -949,7 +969,7 @@
         <v>43</v>
       </c>
     </row>
-    <row r="16" spans="1:3">
+    <row r="16" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A16" t="s">
         <v>44</v>
       </c>
@@ -960,7 +980,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="17" spans="1:3">
+    <row r="17" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A17" t="s">
         <v>47</v>
       </c>
@@ -971,7 +991,7 @@
         <v>49</v>
       </c>
     </row>
-    <row r="18" spans="1:3">
+    <row r="18" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A18" t="s">
         <v>50</v>
       </c>
@@ -982,7 +1002,7 @@
         <v>52</v>
       </c>
     </row>
-    <row r="19" spans="1:3">
+    <row r="19" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A19" t="s">
         <v>53</v>
       </c>
@@ -993,7 +1013,7 @@
         <v>55</v>
       </c>
     </row>
-    <row r="20" spans="1:3">
+    <row r="20" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A20" t="s">
         <v>56</v>
       </c>
@@ -1004,7 +1024,7 @@
         <v>58</v>
       </c>
     </row>
-    <row r="21" spans="1:3">
+    <row r="21" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A21" t="s">
         <v>59</v>
       </c>
@@ -1015,7 +1035,7 @@
         <v>61</v>
       </c>
     </row>
-    <row r="22" spans="1:3">
+    <row r="22" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A22" t="s">
         <v>62</v>
       </c>
@@ -1026,7 +1046,7 @@
         <v>64</v>
       </c>
     </row>
-    <row r="23" spans="1:3">
+    <row r="23" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A23" t="s">
         <v>65</v>
       </c>
@@ -1037,7 +1057,7 @@
         <v>67</v>
       </c>
     </row>
-    <row r="24" spans="1:3">
+    <row r="24" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A24" t="s">
         <v>68</v>
       </c>
@@ -1048,7 +1068,7 @@
         <v>70</v>
       </c>
     </row>
-    <row r="25" spans="1:3">
+    <row r="25" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A25" t="s">
         <v>71</v>
       </c>
@@ -1059,7 +1079,7 @@
         <v>73</v>
       </c>
     </row>
-    <row r="26" spans="1:3">
+    <row r="26" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A26" t="s">
         <v>74</v>
       </c>
@@ -1070,7 +1090,7 @@
         <v>75</v>
       </c>
     </row>
-    <row r="27" spans="1:3">
+    <row r="27" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A27" t="s">
         <v>76</v>
       </c>
@@ -1081,7 +1101,7 @@
         <v>78</v>
       </c>
     </row>
-    <row r="28" spans="1:3">
+    <row r="28" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A28" t="s">
         <v>79</v>
       </c>
@@ -1092,7 +1112,7 @@
         <v>81</v>
       </c>
     </row>
-    <row r="29" spans="1:3">
+    <row r="29" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A29" t="s">
         <v>82</v>
       </c>
@@ -1103,7 +1123,7 @@
         <v>84</v>
       </c>
     </row>
-    <row r="30" spans="1:3">
+    <row r="30" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A30" t="s">
         <v>85</v>
       </c>
@@ -1114,7 +1134,7 @@
         <v>87</v>
       </c>
     </row>
-    <row r="31" spans="1:3">
+    <row r="31" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A31" t="s">
         <v>88</v>
       </c>
@@ -1125,7 +1145,7 @@
         <v>90</v>
       </c>
     </row>
-    <row r="32" spans="1:3">
+    <row r="32" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A32" t="s">
         <v>91</v>
       </c>
@@ -1136,7 +1156,7 @@
         <v>93</v>
       </c>
     </row>
-    <row r="33" spans="1:3">
+    <row r="33" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A33" t="s">
         <v>94</v>
       </c>
@@ -1147,7 +1167,7 @@
         <v>96</v>
       </c>
     </row>
-    <row r="34" spans="1:3">
+    <row r="34" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A34" t="s">
         <v>97</v>
       </c>
@@ -1158,7 +1178,7 @@
         <v>99</v>
       </c>
     </row>
-    <row r="35" spans="1:3">
+    <row r="35" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A35" t="s">
         <v>100</v>
       </c>
@@ -1169,7 +1189,7 @@
         <v>101</v>
       </c>
     </row>
-    <row r="36" spans="1:3">
+    <row r="36" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A36" t="s">
         <v>102</v>
       </c>
@@ -1180,7 +1200,7 @@
         <v>104</v>
       </c>
     </row>
-    <row r="37" spans="1:3">
+    <row r="37" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A37" t="s">
         <v>105</v>
       </c>
@@ -1191,7 +1211,7 @@
         <v>106</v>
       </c>
     </row>
-    <row r="38" spans="1:3">
+    <row r="38" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A38" t="s">
         <v>107</v>
       </c>
@@ -1202,7 +1222,7 @@
         <v>109</v>
       </c>
     </row>
-    <row r="39" spans="1:3">
+    <row r="39" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A39" t="s">
         <v>110</v>
       </c>
@@ -1213,7 +1233,7 @@
         <v>111</v>
       </c>
     </row>
-    <row r="40" spans="1:3">
+    <row r="40" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A40" t="s">
         <v>112</v>
       </c>
@@ -1224,7 +1244,7 @@
         <v>113</v>
       </c>
     </row>
-    <row r="41" spans="1:3">
+    <row r="41" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A41" t="s">
         <v>114</v>
       </c>
@@ -1235,7 +1255,7 @@
         <v>115</v>
       </c>
     </row>
-    <row r="42" spans="1:3">
+    <row r="42" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A42" t="s">
         <v>116</v>
       </c>
@@ -1246,7 +1266,7 @@
         <v>117</v>
       </c>
     </row>
-    <row r="43" spans="1:3">
+    <row r="43" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A43" t="s">
         <v>118</v>
       </c>
@@ -1257,7 +1277,7 @@
         <v>120</v>
       </c>
     </row>
-    <row r="44" spans="1:3">
+    <row r="44" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A44" t="s">
         <v>121</v>
       </c>
@@ -1268,7 +1288,7 @@
         <v>123</v>
       </c>
     </row>
-    <row r="45" spans="1:3">
+    <row r="45" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A45" t="s">
         <v>124</v>
       </c>
@@ -1279,7 +1299,7 @@
         <v>126</v>
       </c>
     </row>
-    <row r="46" spans="1:3">
+    <row r="46" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A46" t="s">
         <v>127</v>
       </c>
@@ -1290,7 +1310,7 @@
         <v>129</v>
       </c>
     </row>
-    <row r="47" spans="1:3">
+    <row r="47" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A47" t="s">
         <v>130</v>
       </c>
@@ -1301,7 +1321,7 @@
         <v>132</v>
       </c>
     </row>
-    <row r="48" spans="1:3">
+    <row r="48" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A48" t="s">
         <v>133</v>
       </c>
@@ -1312,7 +1332,7 @@
         <v>135</v>
       </c>
     </row>
-    <row r="49" spans="1:3">
+    <row r="49" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A49" t="s">
         <v>136</v>
       </c>
@@ -1323,7 +1343,7 @@
         <v>138</v>
       </c>
     </row>
-    <row r="50" spans="1:3">
+    <row r="50" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A50" t="s">
         <v>139</v>
       </c>
@@ -1335,6 +1355,9 @@
       </c>
     </row>
   </sheetData>
-  <pageMargins bottom="1" footer="0.5" header="0.5" left="0.75" right="0.75" top="1"/>
+  <hyperlinks>
+    <hyperlink ref="C2" r:id="rId1" xr:uid="{10CD2F11-CBA7-4471-A237-3EBA9A3E54CB}"/>
+  </hyperlinks>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
v1.0.0 - Fixed: Exclude 中国美术学院 to write to the excel - ADD: Function get_link(school_name) - ADD: Function get_admission_guide(link) - ADD: Function parse_admission_guide(html) - ADD: Function write_admission_guide_to_cvs()
</commit_message>
<xml_diff>
--- a/浙江省2019年三位一体招生信息.xlsx
+++ b/浙江省2019年三位一体招生信息.xlsx
@@ -1,26 +1,21 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="21001"/>
+<workbook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <workbookPr/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Vanad\OneDrive\Documents\Computer Science\Python\Projects\2019-zhejiang-universities-admission-info-scraper\"/>
-    </mc:Choice>
-  </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="1" documentId="11_083E72B50EBA80104345557E01FB694A8904A63C" xr6:coauthVersionLast="38" xr6:coauthVersionMax="38" xr10:uidLastSave="{56898ED1-A20A-4BCB-9195-8D1D41F5DCED}"/>
+  <workbookProtection/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="22500" windowHeight="12330" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView activeTab="0" autoFilterDateGrouping="1" firstSheet="0" minimized="0" showHorizontalScroll="1" showSheetTabs="1" showVerticalScroll="1" tabRatio="600" visibility="visible"/>
   </bookViews>
   <sheets>
-    <sheet name="报考简章" sheetId="1" r:id="rId1"/>
+    <sheet name="报考简章" sheetId="1" state="visible" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="0"/>
+  <definedNames/>
+  <calcPr calcId="124519" fullCalcOnLoad="1"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="150" uniqueCount="142">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="139">
   <si>
     <t>高校名单</t>
   </si>
@@ -29,15 +24,6 @@
   </si>
   <si>
     <t>招生简章</t>
-  </si>
-  <si>
-    <t>中国美术学院</t>
-  </si>
-  <si>
-    <t>1月3日—1月8日</t>
-  </si>
-  <si>
-    <t>http://gaokao.eol.cn/zhe_jiang/dongtai/201802/t20180206_1584734.shtml</t>
   </si>
   <si>
     <t>浙江工业大学</t>
@@ -451,27 +437,20 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="2" x14ac:knownFonts="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <numFmts count="0"/>
+  <fonts count="1">
     <font>
-      <sz val="11"/>
-      <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <u/>
+      <color theme="1"/>
       <sz val="11"/>
-      <color theme="10"/>
-      <name val="Calibri"/>
-      <family val="2"/>
       <scheme val="minor"/>
     </font>
   </fonts>
   <fills count="2">
     <fill>
-      <patternFill patternType="none"/>
+      <patternFill/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
@@ -486,28 +465,16 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="2">
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+  <cellStyleXfs count="1">
+    <xf borderId="0" fillId="0" fontId="0" numFmtId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1"/>
+  <cellXfs count="1">
+    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
   </cellXfs>
-  <cellStyles count="2">
-    <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
-    <cellStyle name="Normal" xfId="0" builtinId="0"/>
+  <cellStyles count="1">
+    <cellStyle builtinId="0" hidden="0" name="Normal" xfId="0"/>
   </cellStyles>
-  <dxfs count="0"/>
-  <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
-  <extLst>
-    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
-      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
-    </ext>
-    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
-      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
-    </ext>
-  </extLst>
+  <tableStyles count="0" defaultPivotStyle="PivotStyleLight16" defaultTableStyle="TableStyleMedium9"/>
 </styleSheet>
 </file>
 
@@ -795,16 +762,20 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:C50"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
+  <dimension ref="A1:C49"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C2" sqref="C2"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="1" spans="1:3">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -815,18 +786,18 @@
         <v>2</v>
       </c>
     </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="2" spans="1:3">
       <c r="A2" t="s">
         <v>3</v>
       </c>
       <c r="B2" t="s">
         <v>4</v>
       </c>
-      <c r="C2" s="1" t="s">
+      <c r="C2" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="3" spans="1:3">
       <c r="A3" t="s">
         <v>6</v>
       </c>
@@ -837,7 +808,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="4" spans="1:3">
       <c r="A4" t="s">
         <v>9</v>
       </c>
@@ -848,7 +819,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="5" spans="1:3">
       <c r="A5" t="s">
         <v>12</v>
       </c>
@@ -859,7 +830,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="6" spans="1:3">
       <c r="A6" t="s">
         <v>15</v>
       </c>
@@ -870,7 +841,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="7" spans="1:3">
       <c r="A7" t="s">
         <v>18</v>
       </c>
@@ -881,7 +852,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="8" spans="1:3">
       <c r="A8" t="s">
         <v>21</v>
       </c>
@@ -892,7 +863,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="9" spans="1:3">
       <c r="A9" t="s">
         <v>24</v>
       </c>
@@ -903,29 +874,29 @@
         <v>26</v>
       </c>
     </row>
-    <row r="10" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="10" spans="1:3">
       <c r="A10" t="s">
         <v>27</v>
       </c>
       <c r="B10" t="s">
+        <v>4</v>
+      </c>
+      <c r="C10" t="s">
         <v>28</v>
       </c>
-      <c r="C10" t="s">
+    </row>
+    <row r="11" spans="1:3">
+      <c r="A11" t="s">
         <v>29</v>
       </c>
-    </row>
-    <row r="11" spans="1:3" x14ac:dyDescent="0.45">
-      <c r="A11" t="s">
+      <c r="B11" t="s">
         <v>30</v>
-      </c>
-      <c r="B11" t="s">
-        <v>7</v>
       </c>
       <c r="C11" t="s">
         <v>31</v>
       </c>
     </row>
-    <row r="12" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="12" spans="1:3">
       <c r="A12" t="s">
         <v>32</v>
       </c>
@@ -936,7 +907,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="13" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="13" spans="1:3">
       <c r="A13" t="s">
         <v>35</v>
       </c>
@@ -947,7 +918,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="14" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="14" spans="1:3">
       <c r="A14" t="s">
         <v>38</v>
       </c>
@@ -958,7 +929,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="15" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="15" spans="1:3">
       <c r="A15" t="s">
         <v>41</v>
       </c>
@@ -969,7 +940,7 @@
         <v>43</v>
       </c>
     </row>
-    <row r="16" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="16" spans="1:3">
       <c r="A16" t="s">
         <v>44</v>
       </c>
@@ -980,7 +951,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="17" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="17" spans="1:3">
       <c r="A17" t="s">
         <v>47</v>
       </c>
@@ -991,7 +962,7 @@
         <v>49</v>
       </c>
     </row>
-    <row r="18" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="18" spans="1:3">
       <c r="A18" t="s">
         <v>50</v>
       </c>
@@ -1002,7 +973,7 @@
         <v>52</v>
       </c>
     </row>
-    <row r="19" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="19" spans="1:3">
       <c r="A19" t="s">
         <v>53</v>
       </c>
@@ -1013,7 +984,7 @@
         <v>55</v>
       </c>
     </row>
-    <row r="20" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="20" spans="1:3">
       <c r="A20" t="s">
         <v>56</v>
       </c>
@@ -1024,7 +995,7 @@
         <v>58</v>
       </c>
     </row>
-    <row r="21" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="21" spans="1:3">
       <c r="A21" t="s">
         <v>59</v>
       </c>
@@ -1035,7 +1006,7 @@
         <v>61</v>
       </c>
     </row>
-    <row r="22" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="22" spans="1:3">
       <c r="A22" t="s">
         <v>62</v>
       </c>
@@ -1046,7 +1017,7 @@
         <v>64</v>
       </c>
     </row>
-    <row r="23" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="23" spans="1:3">
       <c r="A23" t="s">
         <v>65</v>
       </c>
@@ -1057,7 +1028,7 @@
         <v>67</v>
       </c>
     </row>
-    <row r="24" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="24" spans="1:3">
       <c r="A24" t="s">
         <v>68</v>
       </c>
@@ -1068,29 +1039,29 @@
         <v>70</v>
       </c>
     </row>
-    <row r="25" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="25" spans="1:3">
       <c r="A25" t="s">
         <v>71</v>
       </c>
       <c r="B25" t="s">
+        <v>33</v>
+      </c>
+      <c r="C25" t="s">
         <v>72</v>
       </c>
-      <c r="C25" t="s">
+    </row>
+    <row r="26" spans="1:3">
+      <c r="A26" t="s">
         <v>73</v>
       </c>
-    </row>
-    <row r="26" spans="1:3" x14ac:dyDescent="0.45">
-      <c r="A26" t="s">
+      <c r="B26" t="s">
         <v>74</v>
-      </c>
-      <c r="B26" t="s">
-        <v>36</v>
       </c>
       <c r="C26" t="s">
         <v>75</v>
       </c>
     </row>
-    <row r="27" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="27" spans="1:3">
       <c r="A27" t="s">
         <v>76</v>
       </c>
@@ -1101,7 +1072,7 @@
         <v>78</v>
       </c>
     </row>
-    <row r="28" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="28" spans="1:3">
       <c r="A28" t="s">
         <v>79</v>
       </c>
@@ -1112,7 +1083,7 @@
         <v>81</v>
       </c>
     </row>
-    <row r="29" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="29" spans="1:3">
       <c r="A29" t="s">
         <v>82</v>
       </c>
@@ -1123,7 +1094,7 @@
         <v>84</v>
       </c>
     </row>
-    <row r="30" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="30" spans="1:3">
       <c r="A30" t="s">
         <v>85</v>
       </c>
@@ -1134,7 +1105,7 @@
         <v>87</v>
       </c>
     </row>
-    <row r="31" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="31" spans="1:3">
       <c r="A31" t="s">
         <v>88</v>
       </c>
@@ -1145,7 +1116,7 @@
         <v>90</v>
       </c>
     </row>
-    <row r="32" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="32" spans="1:3">
       <c r="A32" t="s">
         <v>91</v>
       </c>
@@ -1156,7 +1127,7 @@
         <v>93</v>
       </c>
     </row>
-    <row r="33" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="33" spans="1:3">
       <c r="A33" t="s">
         <v>94</v>
       </c>
@@ -1167,106 +1138,106 @@
         <v>96</v>
       </c>
     </row>
-    <row r="34" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="34" spans="1:3">
       <c r="A34" t="s">
         <v>97</v>
       </c>
       <c r="B34" t="s">
+        <v>22</v>
+      </c>
+      <c r="C34" t="s">
         <v>98</v>
       </c>
-      <c r="C34" t="s">
+    </row>
+    <row r="35" spans="1:3">
+      <c r="A35" t="s">
         <v>99</v>
       </c>
-    </row>
-    <row r="35" spans="1:3" x14ac:dyDescent="0.45">
-      <c r="A35" t="s">
+      <c r="B35" t="s">
         <v>100</v>
-      </c>
-      <c r="B35" t="s">
-        <v>25</v>
       </c>
       <c r="C35" t="s">
         <v>101</v>
       </c>
     </row>
-    <row r="36" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="36" spans="1:3">
       <c r="A36" t="s">
         <v>102</v>
       </c>
       <c r="B36" t="s">
+        <v>4</v>
+      </c>
+      <c r="C36" t="s">
         <v>103</v>
       </c>
-      <c r="C36" t="s">
+    </row>
+    <row r="37" spans="1:3">
+      <c r="A37" t="s">
         <v>104</v>
       </c>
-    </row>
-    <row r="37" spans="1:3" x14ac:dyDescent="0.45">
-      <c r="A37" t="s">
+      <c r="B37" t="s">
         <v>105</v>
-      </c>
-      <c r="B37" t="s">
-        <v>7</v>
       </c>
       <c r="C37" t="s">
         <v>106</v>
       </c>
     </row>
-    <row r="38" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="38" spans="1:3">
       <c r="A38" t="s">
         <v>107</v>
       </c>
       <c r="B38" t="s">
+        <v>33</v>
+      </c>
+      <c r="C38" t="s">
         <v>108</v>
       </c>
-      <c r="C38" t="s">
+    </row>
+    <row r="39" spans="1:3">
+      <c r="A39" t="s">
         <v>109</v>
       </c>
-    </row>
-    <row r="39" spans="1:3" x14ac:dyDescent="0.45">
-      <c r="A39" t="s">
+      <c r="B39" t="s">
+        <v>22</v>
+      </c>
+      <c r="C39" t="s">
         <v>110</v>
       </c>
-      <c r="B39" t="s">
-        <v>36</v>
-      </c>
-      <c r="C39" t="s">
+    </row>
+    <row r="40" spans="1:3">
+      <c r="A40" t="s">
         <v>111</v>
       </c>
-    </row>
-    <row r="40" spans="1:3" x14ac:dyDescent="0.45">
-      <c r="A40" t="s">
+      <c r="B40" t="s">
+        <v>30</v>
+      </c>
+      <c r="C40" t="s">
         <v>112</v>
       </c>
-      <c r="B40" t="s">
-        <v>25</v>
-      </c>
-      <c r="C40" t="s">
+    </row>
+    <row r="41" spans="1:3">
+      <c r="A41" t="s">
         <v>113</v>
-      </c>
-    </row>
-    <row r="41" spans="1:3" x14ac:dyDescent="0.45">
-      <c r="A41" t="s">
-        <v>114</v>
       </c>
       <c r="B41" t="s">
         <v>33</v>
       </c>
       <c r="C41" t="s">
+        <v>114</v>
+      </c>
+    </row>
+    <row r="42" spans="1:3">
+      <c r="A42" t="s">
         <v>115</v>
       </c>
-    </row>
-    <row r="42" spans="1:3" x14ac:dyDescent="0.45">
-      <c r="A42" t="s">
+      <c r="B42" t="s">
         <v>116</v>
-      </c>
-      <c r="B42" t="s">
-        <v>36</v>
       </c>
       <c r="C42" t="s">
         <v>117</v>
       </c>
     </row>
-    <row r="43" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="43" spans="1:3">
       <c r="A43" t="s">
         <v>118</v>
       </c>
@@ -1277,7 +1248,7 @@
         <v>120</v>
       </c>
     </row>
-    <row r="44" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="44" spans="1:3">
       <c r="A44" t="s">
         <v>121</v>
       </c>
@@ -1288,7 +1259,7 @@
         <v>123</v>
       </c>
     </row>
-    <row r="45" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="45" spans="1:3">
       <c r="A45" t="s">
         <v>124</v>
       </c>
@@ -1299,7 +1270,7 @@
         <v>126</v>
       </c>
     </row>
-    <row r="46" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="46" spans="1:3">
       <c r="A46" t="s">
         <v>127</v>
       </c>
@@ -1310,7 +1281,7 @@
         <v>129</v>
       </c>
     </row>
-    <row r="47" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="47" spans="1:3">
       <c r="A47" t="s">
         <v>130</v>
       </c>
@@ -1321,7 +1292,7 @@
         <v>132</v>
       </c>
     </row>
-    <row r="48" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="48" spans="1:3">
       <c r="A48" t="s">
         <v>133</v>
       </c>
@@ -1332,7 +1303,7 @@
         <v>135</v>
       </c>
     </row>
-    <row r="49" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="49" spans="1:3">
       <c r="A49" t="s">
         <v>136</v>
       </c>
@@ -1343,21 +1314,7 @@
         <v>138</v>
       </c>
     </row>
-    <row r="50" spans="1:3" x14ac:dyDescent="0.45">
-      <c r="A50" t="s">
-        <v>139</v>
-      </c>
-      <c r="B50" t="s">
-        <v>140</v>
-      </c>
-      <c r="C50" t="s">
-        <v>141</v>
-      </c>
-    </row>
   </sheetData>
-  <hyperlinks>
-    <hyperlink ref="C2" r:id="rId1" xr:uid="{10CD2F11-CBA7-4471-A237-3EBA9A3E54CB}"/>
-  </hyperlinks>
-  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+  <pageMargins bottom="1" footer="0.5" header="0.5" left="0.75" right="0.75" top="1"/>
 </worksheet>
 </file>
</xml_diff>